<commit_message>
Adding Linked list program, permutation and recursion comparisons.
Signed-off-by: koa2019 <no-reply>
</commit_message>
<xml_diff>
--- a/lab/lab3_BigOhOmegaTheta_spreadsheet/df_BigOhOmegaThetaExample1and2_v3.xlsx
+++ b/lab/lab3_BigOhOmegaTheta_spreadsheet/df_BigOhOmegaThetaExample1and2_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanYell\Documents\cis17c_fall2023\git_cis17c\lab\lab3_BigOhOmegaTheta_spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0131D4-43FA-4AA4-8BD6-5A95C730774B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A4173A-BAC5-401D-9889-8F58314C78F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="df_fn1" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,6 @@
     <sheet name="lehr_ex2" sheetId="4" r:id="rId6"/>
     <sheet name="lehr_ex1" sheetId="3" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -8287,439 +8284,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="markSort"/>
-      <sheetName val="markSort (2)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="12">
-          <cell r="I12" t="str">
-            <v>Big Omega</v>
-          </cell>
-          <cell r="J12" t="str">
-            <v>Big Oh</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="I13" t="str">
-            <v>Lower Bound</v>
-          </cell>
-          <cell r="J13" t="str">
-            <v>Upper Bound</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="I14" t="str">
-            <v>c'g(n)</v>
-          </cell>
-          <cell r="J14" t="str">
-            <v>c''g(n)</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>25000</v>
-          </cell>
-          <cell r="B15">
-            <v>2</v>
-          </cell>
-          <cell r="F15">
-            <v>25000</v>
-          </cell>
-          <cell r="I15">
-            <v>2187500000</v>
-          </cell>
-          <cell r="J15">
-            <v>1.940625</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>50000</v>
-          </cell>
-          <cell r="B16">
-            <v>8</v>
-          </cell>
-          <cell r="F16">
-            <v>50000</v>
-          </cell>
-          <cell r="I16">
-            <v>8750000000</v>
-          </cell>
-          <cell r="J16">
-            <v>7.7625000000000002</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>100000</v>
-          </cell>
-          <cell r="B17">
-            <v>31</v>
-          </cell>
-          <cell r="F17">
-            <v>100000</v>
-          </cell>
-          <cell r="I17">
-            <v>35000000000</v>
-          </cell>
-          <cell r="J17">
-            <v>31.05</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>200000</v>
-          </cell>
-          <cell r="B18">
-            <v>124</v>
-          </cell>
-          <cell r="F18">
-            <v>200000</v>
-          </cell>
-          <cell r="I18">
-            <v>140000000000</v>
-          </cell>
-          <cell r="J18">
-            <v>124.2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="12">
-          <cell r="K12" t="str">
-            <v>Big Omega</v>
-          </cell>
-          <cell r="L12" t="str">
-            <v>Big Oh</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="K13" t="str">
-            <v>Lower Bound</v>
-          </cell>
-          <cell r="L13" t="str">
-            <v>Upper Bound</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="I14" t="str">
-            <v>f(n)</v>
-          </cell>
-          <cell r="K14" t="str">
-            <v>c'g(n)</v>
-          </cell>
-          <cell r="L14" t="str">
-            <v>c''g(n)</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>25000</v>
-          </cell>
-          <cell r="B15">
-            <v>4</v>
-          </cell>
-          <cell r="F15">
-            <v>25000</v>
-          </cell>
-          <cell r="I15">
-            <v>25002.940624999999</v>
-          </cell>
-          <cell r="K15">
-            <v>2187500000</v>
-          </cell>
-          <cell r="L15">
-            <v>1.940625</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>30000</v>
-          </cell>
-          <cell r="B16">
-            <v>9</v>
-          </cell>
-          <cell r="F16">
-            <v>30000</v>
-          </cell>
-          <cell r="I16">
-            <v>30003.7945</v>
-          </cell>
-          <cell r="K16">
-            <v>3150000000</v>
-          </cell>
-          <cell r="L16">
-            <v>2.7944999999999998</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>35000</v>
-          </cell>
-          <cell r="B17">
-            <v>11</v>
-          </cell>
-          <cell r="F17">
-            <v>35000</v>
-          </cell>
-          <cell r="I17">
-            <v>35004.803625</v>
-          </cell>
-          <cell r="K17">
-            <v>4287500000</v>
-          </cell>
-          <cell r="L17">
-            <v>3.8036249999999998</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>40000</v>
-          </cell>
-          <cell r="B18">
-            <v>11</v>
-          </cell>
-          <cell r="F18">
-            <v>40000</v>
-          </cell>
-          <cell r="I18">
-            <v>40005.968000000001</v>
-          </cell>
-          <cell r="K18">
-            <v>5600000000</v>
-          </cell>
-          <cell r="L18">
-            <v>4.968</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>45000</v>
-          </cell>
-          <cell r="B19">
-            <v>16</v>
-          </cell>
-          <cell r="F19">
-            <v>45000</v>
-          </cell>
-          <cell r="I19">
-            <v>45007.287624999997</v>
-          </cell>
-          <cell r="K19">
-            <v>7087500000</v>
-          </cell>
-          <cell r="L19">
-            <v>6.2876250000000002</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>50000</v>
-          </cell>
-          <cell r="B20">
-            <v>16</v>
-          </cell>
-          <cell r="F20">
-            <v>50000</v>
-          </cell>
-          <cell r="I20">
-            <v>50008.762499999997</v>
-          </cell>
-          <cell r="K20">
-            <v>8750000000</v>
-          </cell>
-          <cell r="L20">
-            <v>7.7625000000000002</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>55000</v>
-          </cell>
-          <cell r="B21">
-            <v>21</v>
-          </cell>
-          <cell r="F21">
-            <v>55000</v>
-          </cell>
-          <cell r="I21">
-            <v>55010.392625</v>
-          </cell>
-          <cell r="K21">
-            <v>10587500000</v>
-          </cell>
-          <cell r="L21">
-            <v>9.3926250000000007</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>60000</v>
-          </cell>
-          <cell r="B22">
-            <v>28</v>
-          </cell>
-          <cell r="F22">
-            <v>60000</v>
-          </cell>
-          <cell r="I22">
-            <v>60012.178</v>
-          </cell>
-          <cell r="K22">
-            <v>12600000000</v>
-          </cell>
-          <cell r="L22">
-            <v>11.177999999999999</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>65000</v>
-          </cell>
-          <cell r="B23">
-            <v>44</v>
-          </cell>
-          <cell r="F23">
-            <v>65000</v>
-          </cell>
-          <cell r="I23">
-            <v>65014.118625000003</v>
-          </cell>
-          <cell r="K23">
-            <v>14787500000</v>
-          </cell>
-          <cell r="L23">
-            <v>13.118625</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>70000</v>
-          </cell>
-          <cell r="B24">
-            <v>85</v>
-          </cell>
-          <cell r="F24">
-            <v>70000</v>
-          </cell>
-          <cell r="I24">
-            <v>70016.214500000002</v>
-          </cell>
-          <cell r="K24">
-            <v>17150000000</v>
-          </cell>
-          <cell r="L24">
-            <v>15.214499999999999</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>75000</v>
-          </cell>
-          <cell r="B25">
-            <v>123</v>
-          </cell>
-          <cell r="F25">
-            <v>75000</v>
-          </cell>
-          <cell r="I25">
-            <v>75018.465624999997</v>
-          </cell>
-          <cell r="K25">
-            <v>19687500000</v>
-          </cell>
-          <cell r="L25">
-            <v>17.465624999999999</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>80000</v>
-          </cell>
-          <cell r="B26">
-            <v>170</v>
-          </cell>
-          <cell r="F26">
-            <v>80000</v>
-          </cell>
-          <cell r="I26">
-            <v>80020.872000000003</v>
-          </cell>
-          <cell r="K26">
-            <v>22400000000</v>
-          </cell>
-          <cell r="L26">
-            <v>19.872</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>85000</v>
-          </cell>
-          <cell r="B27">
-            <v>209</v>
-          </cell>
-          <cell r="F27">
-            <v>85000</v>
-          </cell>
-          <cell r="I27">
-            <v>85023.433625000005</v>
-          </cell>
-          <cell r="K27">
-            <v>25287500000</v>
-          </cell>
-          <cell r="L27">
-            <v>22.433624999999999</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>90000</v>
-          </cell>
-          <cell r="B28">
-            <v>518</v>
-          </cell>
-          <cell r="F28">
-            <v>90000</v>
-          </cell>
-          <cell r="I28">
-            <v>90026.150500000003</v>
-          </cell>
-          <cell r="K28">
-            <v>28350000000</v>
-          </cell>
-          <cell r="L28">
-            <v>25.150500000000001</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>95000</v>
-          </cell>
-          <cell r="B29">
-            <v>879</v>
-          </cell>
-          <cell r="F29">
-            <v>95000</v>
-          </cell>
-          <cell r="I29">
-            <v>95029.022624999998</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -9019,11 +8583,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.77734375" customWidth="1"/>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
@@ -9039,7 +8603,7 @@
     <col min="14" max="1024" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
         <v>50</v>
       </c>
@@ -9055,7 +8619,7 @@
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
@@ -9071,14 +8635,14 @@
       <c r="L2" s="53"/>
       <c r="M2" s="53"/>
     </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
       <c r="F3" s="30"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -9092,7 +8656,7 @@
       <c r="E4" s="54"/>
       <c r="F4" s="30"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -9113,7 +8677,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
@@ -9129,7 +8693,7 @@
       <c r="F6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
@@ -9146,7 +8710,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>19</v>
@@ -9163,7 +8727,7 @@
       <c r="G8" s="52"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -9180,7 +8744,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -9198,7 +8762,7 @@
       </c>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -9209,7 +8773,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -9220,7 +8784,7 @@
       <c r="I12" s="34"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:13" s="44" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" s="44" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
@@ -9235,7 +8799,7 @@
       </c>
       <c r="J13" s="45"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="17" t="s">
@@ -9254,7 +8818,7 @@
       </c>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
@@ -9281,7 +8845,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -9300,7 +8864,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16:F35" si="2">$D$8*C16+$D$9*B16</f>
+        <f>$D$8*C16+$D$9*B16</f>
         <v>45</v>
       </c>
       <c r="G16" s="3"/>
@@ -9313,7 +8877,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -9332,7 +8896,7 @@
         <v>8</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F16:F35" si="2">$D$8*C17+$D$9*B17</f>
         <v>75</v>
       </c>
       <c r="G17" s="3"/>
@@ -9345,7 +8909,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -9377,7 +8941,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>4</v>
       </c>
@@ -9409,7 +8973,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -9441,7 +9005,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>6</v>
       </c>
@@ -9473,7 +9037,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>7</v>
       </c>
@@ -9505,7 +9069,7 @@
         <v>262.5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>8</v>
       </c>
@@ -9537,7 +9101,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>9</v>
       </c>
@@ -9569,7 +9133,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>10</v>
       </c>
@@ -9601,7 +9165,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -9633,7 +9197,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>12</v>
       </c>
@@ -9665,7 +9229,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>13</v>
       </c>
@@ -9697,7 +9261,7 @@
         <v>487.5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>14</v>
       </c>
@@ -9729,7 +9293,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>15</v>
       </c>
@@ -9761,7 +9325,7 @@
         <v>562.5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>16</v>
       </c>
@@ -9793,7 +9357,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -9825,7 +9389,7 @@
         <v>637.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>18</v>
       </c>
@@ -9857,7 +9421,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>19</v>
       </c>
@@ -9889,7 +9453,7 @@
         <v>712.5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>20</v>
       </c>
@@ -9942,11 +9506,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
@@ -9962,7 +9526,7 @@
     <col min="14" max="1024" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
         <v>50</v>
       </c>
@@ -9978,7 +9542,7 @@
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
@@ -9994,7 +9558,7 @@
       <c r="L2" s="53"/>
       <c r="M2" s="53"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
@@ -10008,7 +9572,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -10022,7 +9586,7 @@
       <c r="E4" s="55"/>
       <c r="F4" s="30"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="38" t="s">
@@ -10039,7 +9603,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
@@ -10055,7 +9619,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
@@ -10069,7 +9633,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>19</v>
@@ -10085,7 +9649,7 @@
       </c>
       <c r="G8" s="52"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -10102,7 +9666,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -10120,7 +9684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -10131,7 +9695,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -10143,7 +9707,7 @@
       </c>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -10157,7 +9721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="17" t="s">
@@ -10175,7 +9739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
@@ -10202,7 +9766,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -10234,7 +9798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -10266,7 +9830,7 @@
         <v>16.707164759350956</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -10298,7 +9862,7 @@
         <v>26.480229636941264</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>4</v>
       </c>
@@ -10330,7 +9894,7 @@
         <v>33.414329518701912</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -10362,7 +9926,7 @@
         <v>38.792835240649048</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>6</v>
       </c>
@@ -10394,7 +9958,7 @@
         <v>43.18739439629222</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>7</v>
       </c>
@@ -10426,7 +9990,7 @@
         <v>46.902941220791256</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>8</v>
       </c>
@@ -10458,7 +10022,7 @@
         <v>50.121494278052865</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>9</v>
       </c>
@@ -10490,7 +10054,7 @@
         <v>52.960459273882527</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>10</v>
       </c>
@@ -10522,7 +10086,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -10554,7 +10118,7 @@
         <v>57.797294026281499</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>12</v>
       </c>
@@ -10586,7 +10150,7 @@
         <v>59.894559155643179</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>13</v>
       </c>
@@ -10618,7 +10182,7 @@
         <v>61.823856053029438</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>14</v>
       </c>
@@ -10650,7 +10214,7 @@
         <v>63.610105980142208</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>15</v>
       </c>
@@ -10682,7 +10246,7 @@
         <v>65.273064877590315</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>16</v>
       </c>
@@ -10714,7 +10278,7 @@
         <v>66.828659037403824</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -10746,7 +10310,7 @@
         <v>68.289915136494201</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>18</v>
       </c>
@@ -10778,7 +10342,7 @@
         <v>69.66762403323348</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>19</v>
       </c>
@@ -10810,7 +10374,7 @@
         <v>70.970824852882004</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>20</v>
       </c>
@@ -10866,7 +10430,7 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
@@ -10882,7 +10446,7 @@
     <col min="14" max="1024" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
         <v>51</v>
       </c>
@@ -10898,7 +10462,7 @@
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
@@ -10914,7 +10478,7 @@
       <c r="L2" s="53"/>
       <c r="M2" s="53"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
@@ -10928,7 +10492,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -10942,7 +10506,7 @@
       <c r="E4" s="56"/>
       <c r="F4" s="30"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="38" t="s">
@@ -10959,7 +10523,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
@@ -10975,7 +10539,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
@@ -10991,7 +10555,7 @@
       </c>
       <c r="G7" s="52"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>19</v>
@@ -11015,7 +10579,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -11032,7 +10596,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -11040,7 +10604,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -11051,7 +10615,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -11063,7 +10627,7 @@
       </c>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -11077,7 +10641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="17" t="s">
@@ -11095,7 +10659,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
@@ -11122,7 +10686,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -11154,7 +10718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -11186,7 +10750,7 @@
         <v>27.372332821789627</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -11218,7 +10782,7 @@
         <v>37.257706532672252</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>4</v>
       </c>
@@ -11250,7 +10814,7 @@
         <v>46.427531547319639</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -11282,7 +10846,7 @@
         <v>55.36551775040509</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>6</v>
       </c>
@@ -11314,7 +10878,7 @@
         <v>64.256974149284645</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>7</v>
       </c>
@@ -11346,7 +10910,7 @@
         <v>73.185000054981586</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>8</v>
       </c>
@@ -11378,7 +10942,7 @@
         <v>82.189895032200596</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>9</v>
       </c>
@@ -11410,7 +10974,7 @@
         <v>91.291688629674013</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>10</v>
       </c>
@@ -11442,7 +11006,7 @@
         <v>100.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -11474,7 +11038,7 @@
         <v>109.81880398365639</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>12</v>
       </c>
@@ -11506,7 +11070,7 @@
         <v>119.24890836820055</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>13</v>
       </c>
@@ -11538,7 +11102,7 @@
         <v>128.78931343814338</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>14</v>
       </c>
@@ -11570,7 +11134,7 @@
         <v>138.43798944254624</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>15</v>
       </c>
@@ -11602,7 +11166,7 @@
         <v>148.19233508805593</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>16</v>
       </c>
@@ -11634,7 +11198,7 @@
         <v>158.04945393952386</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -11666,7 +11230,7 @@
         <v>168.00632337338834</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>18</v>
       </c>
@@ -11698,7 +11262,7 @@
         <v>178.05989841291944</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>19</v>
       </c>
@@ -11730,7 +11294,7 @@
         <v>188.20717524906067</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>20</v>
       </c>
@@ -11787,7 +11351,7 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
@@ -11803,7 +11367,7 @@
     <col min="14" max="1024" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
         <v>51</v>
       </c>
@@ -11819,7 +11383,7 @@
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
@@ -11835,7 +11399,7 @@
       <c r="L2" s="53"/>
       <c r="M2" s="53"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
@@ -11849,7 +11413,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -11863,7 +11427,7 @@
       <c r="E4" s="57"/>
       <c r="F4" s="30"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="38" t="s">
@@ -11880,7 +11444,7 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
@@ -11896,7 +11460,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
@@ -11912,7 +11476,7 @@
       </c>
       <c r="G7" s="52"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>19</v>
@@ -11936,7 +11500,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -11953,7 +11517,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -11961,7 +11525,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -11972,7 +11536,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -11984,7 +11548,7 @@
       </c>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -11998,7 +11562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="17" t="s">
@@ -12016,7 +11580,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
@@ -12043,7 +11607,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -12075,7 +11639,7 @@
         <v>50.55</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -12107,7 +11671,7 @@
         <v>97.2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -12139,7 +11703,7 @@
         <v>154.94999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>4</v>
       </c>
@@ -12171,7 +11735,7 @@
         <v>223.8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -12203,7 +11767,7 @@
         <v>303.75</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>6</v>
       </c>
@@ -12235,7 +11799,7 @@
         <v>394.79999999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>7</v>
       </c>
@@ -12267,7 +11831,7 @@
         <v>496.95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>8</v>
       </c>
@@ -12299,7 +11863,7 @@
         <v>610.20000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>9</v>
       </c>
@@ -12331,7 +11895,7 @@
         <v>734.55</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>10</v>
       </c>
@@ -12363,7 +11927,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -12395,7 +11959,7 @@
         <v>1016.55</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>12</v>
       </c>
@@ -12427,7 +11991,7 @@
         <v>1174.1999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>13</v>
       </c>
@@ -12459,7 +12023,7 @@
         <v>1342.9499999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>14</v>
       </c>
@@ -12491,7 +12055,7 @@
         <v>1522.8</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>15</v>
       </c>
@@ -12523,7 +12087,7 @@
         <v>1713.75</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>16</v>
       </c>
@@ -12555,7 +12119,7 @@
         <v>1915.8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -12587,7 +12151,7 @@
         <v>2128.9499999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>18</v>
       </c>
@@ -12619,7 +12183,7 @@
         <v>2353.1999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>19</v>
       </c>
@@ -12651,7 +12215,7 @@
         <v>2588.5500000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>20</v>
       </c>
@@ -12708,7 +12272,7 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.88671875" customWidth="1"/>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
@@ -12721,7 +12285,7 @@
     <col min="14" max="1024" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="53" t="s">
         <v>0</v>
       </c>
@@ -12737,7 +12301,7 @@
       <c r="L1" s="53"/>
       <c r="M1" s="53"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
@@ -12753,7 +12317,7 @@
       <c r="L2" s="53"/>
       <c r="M2" s="53"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
@@ -12767,7 +12331,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -12780,8 +12344,8 @@
       <c r="D4" s="58"/>
       <c r="E4" s="58"/>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -12795,7 +12359,7 @@
       <c r="E6" s="59"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="60"/>
       <c r="B7" s="6" t="s">
         <v>8</v>
@@ -12807,7 +12371,7 @@
       <c r="E7" s="61"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="60"/>
       <c r="B8" s="4" t="s">
         <v>10</v>
@@ -12819,7 +12383,7 @@
       <c r="E8" s="62"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="60"/>
       <c r="B9" s="6" t="s">
         <v>12</v>
@@ -12831,7 +12395,7 @@
       <c r="E9" s="61"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -12845,7 +12409,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -12873,7 +12437,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>17</v>
@@ -12893,7 +12457,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
         <v>19</v>
@@ -12913,7 +12477,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>21</v>
@@ -12933,7 +12497,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -12953,7 +12517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -12967,7 +12531,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -12985,7 +12549,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -13003,7 +12567,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="17" t="s">
@@ -13025,7 +12589,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>32</v>
       </c>
@@ -13064,7 +12628,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>1</v>
       </c>
@@ -13106,7 +12670,7 @@
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2</v>
       </c>
@@ -13148,7 +12712,7 @@
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>3</v>
       </c>
@@ -13190,7 +12754,7 @@
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>4</v>
       </c>
@@ -13232,7 +12796,7 @@
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>5</v>
       </c>
@@ -13274,7 +12838,7 @@
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>6</v>
       </c>
@@ -13316,7 +12880,7 @@
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>7</v>
       </c>
@@ -13358,7 +12922,7 @@
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>8</v>
       </c>
@@ -13400,7 +12964,7 @@
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>9</v>
       </c>
@@ -13442,7 +13006,7 @@
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>10</v>
       </c>
@@ -13484,7 +13048,7 @@
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>11</v>
       </c>
@@ -13526,7 +13090,7 @@
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>12</v>
       </c>
@@ -13568,7 +13132,7 @@
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>13</v>
       </c>
@@ -13610,7 +13174,7 @@
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>14</v>
       </c>
@@ -13652,7 +13216,7 @@
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>15</v>
       </c>
@@ -13694,7 +13258,7 @@
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>16</v>
       </c>
@@ -13736,7 +13300,7 @@
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>17</v>
       </c>
@@ -13778,7 +13342,7 @@
       <c r="L37" s="20"/>
       <c r="M37" s="20"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>18</v>
       </c>
@@ -13820,7 +13384,7 @@
       <c r="L38" s="20"/>
       <c r="M38" s="20"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>19</v>
       </c>
@@ -13862,7 +13426,7 @@
       <c r="L39" s="20"/>
       <c r="M39" s="20"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>20</v>
       </c>
@@ -13931,7 +13495,7 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.44140625" customWidth="1"/>
     <col min="2" max="7" width="9.44140625" style="3" customWidth="1"/>
@@ -13940,7 +13504,7 @@
     <col min="10" max="10" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="53" t="s">
         <v>0</v>
       </c>
@@ -13952,7 +13516,7 @@
       <c r="H2" s="53"/>
       <c r="I2" s="53"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="53" t="s">
         <v>1</v>
       </c>
@@ -13964,7 +13528,7 @@
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -13987,7 +13551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
@@ -13999,7 +13563,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
@@ -14011,7 +13575,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
@@ -14023,7 +13587,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G9" s="10" t="s">
         <v>23</v>
       </c>
@@ -14034,7 +13598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H11" s="13" t="s">
         <v>24</v>
       </c>
@@ -14042,7 +13606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H12" s="15" t="s">
         <v>26</v>
       </c>
@@ -14050,7 +13614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="17" t="s">
         <v>28</v>
       </c>
@@ -14064,7 +13628,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -14090,7 +13654,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -14121,7 +13685,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1</v>
       </c>
@@ -14152,7 +13716,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2</v>
       </c>
@@ -14183,7 +13747,7 @@
         <v>87.75</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>3</v>
       </c>
@@ -14214,7 +13778,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>4</v>
       </c>
@@ -14245,7 +13809,7 @@
         <v>406.25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>5</v>
       </c>
@@ -14276,7 +13840,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>6</v>
       </c>
@@ -14307,7 +13871,7 @@
         <v>1114.75</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>7</v>
       </c>
@@ -14338,7 +13902,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>8</v>
       </c>
@@ -14369,7 +13933,7 @@
         <v>2369.25</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>9</v>
       </c>
@@ -14400,7 +13964,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>10</v>
       </c>
@@ -14431,7 +13995,7 @@
         <v>4325.75</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -14462,7 +14026,7 @@
         <v>5616</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>12</v>
       </c>
@@ -14493,7 +14057,7 @@
         <v>7140.25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>13</v>
       </c>
@@ -14524,7 +14088,7 @@
         <v>8918</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>14</v>
       </c>
@@ -14555,7 +14119,7 @@
         <v>10968.75</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>15</v>
       </c>
@@ -14586,7 +14150,7 @@
         <v>13312</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>16</v>
       </c>
@@ -14617,7 +14181,7 @@
         <v>15967.25</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -14648,7 +14212,7 @@
         <v>18954</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>18</v>
       </c>
@@ -14679,7 +14243,7 @@
         <v>22291.75</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>19</v>
       </c>
@@ -14732,7 +14296,7 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="7" width="9.44140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="3" customWidth="1"/>
@@ -14740,7 +14304,7 @@
     <col min="10" max="10" width="9.44140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -14754,7 +14318,7 @@
       <c r="I2" s="53"/>
       <c r="J2" s="53"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="53" t="s">
         <v>1</v>
       </c>
@@ -14766,7 +14330,7 @@
       <c r="H3" s="53"/>
       <c r="I3" s="53"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -14789,7 +14353,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
@@ -14801,7 +14365,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
@@ -14813,7 +14377,7 @@
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
@@ -14825,7 +14389,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G9" s="25" t="s">
         <v>23</v>
       </c>
@@ -14836,7 +14400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H11" s="13" t="s">
         <v>24</v>
       </c>
@@ -14844,7 +14408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H12" s="15" t="s">
         <v>26</v>
       </c>
@@ -14852,7 +14416,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D13" s="17" t="s">
         <v>28</v>
       </c>
@@ -14866,7 +14430,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -14892,7 +14456,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>1</v>
       </c>
@@ -14923,7 +14487,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2</v>
       </c>
@@ -14942,7 +14506,7 @@
         <v>8</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F15:F34" si="1">$D$5*E16+$D$6*D16+$D$7*C16+$D$8*B16</f>
+        <f t="shared" ref="F16:F34" si="1">$D$5*E16+$D$6*D16+$D$7*C16+$D$8*B16</f>
         <v>-1076</v>
       </c>
       <c r="H16" s="20">
@@ -14950,11 +14514,11 @@
         <v>12</v>
       </c>
       <c r="I16" s="20">
-        <f t="shared" ref="I15:I34" si="3">$H$9*E16</f>
+        <f t="shared" ref="I16:I34" si="3">$H$9*E16</f>
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>3</v>
       </c>
@@ -14965,7 +14529,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" ref="D15:D34" si="4">C17*C17</f>
+        <f t="shared" ref="D17:D34" si="4">C17*C17</f>
         <v>9</v>
       </c>
       <c r="E17" s="3">
@@ -14985,7 +14549,7 @@
         <v>87.75</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>4</v>
       </c>
@@ -15016,7 +14580,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>5</v>
       </c>
@@ -15047,7 +14611,7 @@
         <v>406.25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>6</v>
       </c>
@@ -15078,7 +14642,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>7</v>
       </c>
@@ -15109,7 +14673,7 @@
         <v>1114.75</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>8</v>
       </c>
@@ -15140,7 +14704,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>9</v>
       </c>
@@ -15171,7 +14735,7 @@
         <v>2369.25</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>10</v>
       </c>
@@ -15202,7 +14766,7 @@
         <v>3250</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>11</v>
       </c>
@@ -15233,7 +14797,7 @@
         <v>4325.75</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>12</v>
       </c>
@@ -15264,7 +14828,7 @@
         <v>5616</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>13</v>
       </c>
@@ -15295,7 +14859,7 @@
         <v>7140.25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>14</v>
       </c>
@@ -15326,7 +14890,7 @@
         <v>8918</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>15</v>
       </c>
@@ -15357,7 +14921,7 @@
         <v>10968.75</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>16</v>
       </c>
@@ -15388,7 +14952,7 @@
         <v>13312</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>17</v>
       </c>
@@ -15419,7 +14983,7 @@
         <v>15967.25</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>18</v>
       </c>
@@ -15450,7 +15014,7 @@
         <v>18954</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>19</v>
       </c>
@@ -15481,7 +15045,7 @@
         <v>22291.75</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>20</v>
       </c>

</xml_diff>